<commit_message>
Change color of buses
</commit_message>
<xml_diff>
--- a/shuttle.xlsx
+++ b/shuttle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangwentao/Desktop/浦东公租房/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F246951-6BB6-9A48-A0C2-134CB96CBB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2223943D-31B6-0649-8C5E-0F66E6747915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" xr2:uid="{C9FD647D-2FFF-4BC2-B220-0407C10CAB3A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="246">
   <si>
     <t>1号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -672,6 +672,186 @@
   </si>
   <si>
     <t>黄兴路延吉东路公交站</t>
+  </si>
+  <si>
+    <t>1号</t>
+  </si>
+  <si>
+    <t>中山公园</t>
+  </si>
+  <si>
+    <t>沪FD0815</t>
+  </si>
+  <si>
+    <t>金旅</t>
+  </si>
+  <si>
+    <t>2号</t>
+  </si>
+  <si>
+    <t>梅陇</t>
+  </si>
+  <si>
+    <t>沪FA1511</t>
+  </si>
+  <si>
+    <t>大通</t>
+  </si>
+  <si>
+    <t>3号</t>
+  </si>
+  <si>
+    <t>共富新村</t>
+  </si>
+  <si>
+    <t>沪EP5273</t>
+  </si>
+  <si>
+    <t>4号</t>
+  </si>
+  <si>
+    <t>徐家汇</t>
+  </si>
+  <si>
+    <t>沪FA5278</t>
+  </si>
+  <si>
+    <t>5号</t>
+  </si>
+  <si>
+    <t>川沙</t>
+  </si>
+  <si>
+    <t>沪EQ0268</t>
+  </si>
+  <si>
+    <t>6号</t>
+  </si>
+  <si>
+    <t>徐汇-星中路</t>
+  </si>
+  <si>
+    <t>沪ET0038</t>
+  </si>
+  <si>
+    <t>7号</t>
+  </si>
+  <si>
+    <t>普陀-虹足</t>
+  </si>
+  <si>
+    <t>沪FA7781</t>
+  </si>
+  <si>
+    <t>8号</t>
+  </si>
+  <si>
+    <t>虹口提篮桥</t>
+  </si>
+  <si>
+    <t>沪ES7749</t>
+  </si>
+  <si>
+    <t>9号</t>
+  </si>
+  <si>
+    <t>沪太路(大华)</t>
+  </si>
+  <si>
+    <t>沪EG5617</t>
+  </si>
+  <si>
+    <t>10号</t>
+  </si>
+  <si>
+    <t>浦东周浦</t>
+  </si>
+  <si>
+    <t>沪ER0717</t>
+  </si>
+  <si>
+    <t>11号</t>
+  </si>
+  <si>
+    <t>闵行颛桥</t>
+  </si>
+  <si>
+    <t>沪EL3573</t>
+  </si>
+  <si>
+    <t>12路</t>
+  </si>
+  <si>
+    <t>宝山-中原</t>
+  </si>
+  <si>
+    <t>沪FA8136</t>
+  </si>
+  <si>
+    <t>13路</t>
+  </si>
+  <si>
+    <t>外高桥</t>
+  </si>
+  <si>
+    <t>沪FC8312</t>
+  </si>
+  <si>
+    <t>14路</t>
+  </si>
+  <si>
+    <t>浦东上浦路</t>
+  </si>
+  <si>
+    <t>沪EP0561</t>
+  </si>
+  <si>
+    <t>15号</t>
+  </si>
+  <si>
+    <t>新闸路</t>
+  </si>
+  <si>
+    <t>沪EL2819</t>
+  </si>
+  <si>
+    <t>16号</t>
+  </si>
+  <si>
+    <t>闵行高华小区</t>
+  </si>
+  <si>
+    <t>沪FA7507</t>
+  </si>
+  <si>
+    <t>大巴</t>
+  </si>
+  <si>
+    <t>17号</t>
+  </si>
+  <si>
+    <t>老闵行(翻版)</t>
+  </si>
+  <si>
+    <t>沪EJ5669</t>
+  </si>
+  <si>
+    <t>18号</t>
+  </si>
+  <si>
+    <t>闵行南方(翻版)</t>
+  </si>
+  <si>
+    <t>沪EH1228</t>
+  </si>
+  <si>
+    <t>19号</t>
+  </si>
+  <si>
+    <t>张庙(翻版)</t>
+  </si>
+  <si>
+    <t>沪EB7900</t>
   </si>
 </sst>
 </file>
@@ -762,7 +942,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1080,9 +1260,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF0ACB6-7E1A-4B69-9E58-0C214360D197}">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M15" sqref="M15"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -1136,10 +1316,18 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>189</v>
+      </c>
       <c r="E3" s="3">
         <v>0.30555555555555552</v>
       </c>
@@ -1148,10 +1336,18 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>189</v>
+      </c>
       <c r="E4" s="3">
         <v>0.3125</v>
       </c>
@@ -1180,10 +1376,18 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="A6" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E6" s="3">
         <v>0.29166666666666669</v>
       </c>
@@ -1192,10 +1396,18 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="A7" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E7" s="3">
         <v>0.30555555555555552</v>
       </c>
@@ -1204,10 +1416,18 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="A8" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E8" s="3">
         <v>0.30902777777777779</v>
       </c>
@@ -1216,10 +1436,18 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="A9" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E9" s="3">
         <v>0.3125</v>
       </c>
@@ -1228,10 +1456,18 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="A10" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E10" s="3">
         <v>0.31597222222222221</v>
       </c>
@@ -1260,10 +1496,18 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="A12" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E12" s="3">
         <v>0.29375000000000001</v>
       </c>
@@ -1272,10 +1516,18 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+      <c r="A13" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E13" s="3">
         <v>0.2951388888888889</v>
       </c>
@@ -1284,10 +1536,18 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="A14" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E14" s="3">
         <v>0.2986111111111111</v>
       </c>
@@ -1296,10 +1556,18 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
+      <c r="A15" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E15" s="3">
         <v>0.30208333333333331</v>
       </c>
@@ -1308,10 +1576,18 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+      <c r="A16" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E16" s="3">
         <v>0.30902777777777779</v>
       </c>
@@ -1320,10 +1596,18 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="A17" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E17" s="3">
         <v>0.31944444444444448</v>
       </c>
@@ -1352,10 +1636,18 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="A19" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E19" s="3">
         <v>0.31944444444444448</v>
       </c>
@@ -1364,10 +1656,18 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="A20" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E20" s="3">
         <v>0.32291666666666669</v>
       </c>
@@ -1376,10 +1676,18 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+      <c r="A21" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E21" s="3">
         <v>0.3263888888888889</v>
       </c>
@@ -1388,10 +1696,18 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="A22" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E22" s="3">
         <v>0.33333333333333331</v>
       </c>
@@ -1400,10 +1716,18 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="A23" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E23" s="3">
         <v>0.34027777777777773</v>
       </c>
@@ -1432,10 +1756,18 @@
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="A25" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E25" s="3">
         <v>0.30555555555555552</v>
       </c>
@@ -1444,10 +1776,18 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="A26" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E26" s="3">
         <v>0.3125</v>
       </c>
@@ -1456,10 +1796,18 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="A27" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E27" s="3">
         <v>0.31944444444444448</v>
       </c>
@@ -1468,10 +1816,18 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="A28" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E28" s="3">
         <v>0.3263888888888889</v>
       </c>
@@ -1480,10 +1836,18 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+      <c r="A29" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E29" s="3">
         <v>0.33333333333333331</v>
       </c>
@@ -1512,10 +1876,18 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+      <c r="A31" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E31" s="3">
         <v>0.30555555555555552</v>
       </c>
@@ -1524,10 +1896,18 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="A32" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E32" s="3">
         <v>0.31597222222222221</v>
       </c>
@@ -1536,10 +1916,18 @@
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
+      <c r="A33" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E33" s="3">
         <v>0.31944444444444448</v>
       </c>
@@ -1568,10 +1956,18 @@
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
+      <c r="A35" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E35" s="3">
         <v>0.30555555555555552</v>
       </c>
@@ -1580,10 +1976,18 @@
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
+      <c r="A36" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E36" s="3">
         <v>0.30902777777777779</v>
       </c>
@@ -1592,10 +1996,18 @@
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
+      <c r="A37" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E37" s="3">
         <v>0.3125</v>
       </c>
@@ -1604,10 +2016,18 @@
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
+      <c r="A38" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E38" s="3">
         <v>0.3263888888888889</v>
       </c>
@@ -1616,10 +2036,18 @@
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
+      <c r="A39" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E39" s="3">
         <v>0.3298611111111111</v>
       </c>
@@ -1648,10 +2076,18 @@
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
+      <c r="A41" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E41" s="3">
         <v>0.31944444444444448</v>
       </c>
@@ -1660,10 +2096,18 @@
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
+      <c r="A42" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E42" s="3">
         <v>0.3215277777777778</v>
       </c>
@@ -1672,10 +2116,18 @@
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
+      <c r="A43" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E43" s="3">
         <v>0.32500000000000001</v>
       </c>
@@ -1684,10 +2136,18 @@
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
+      <c r="A44" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E44" s="3">
         <v>0.33333333333333331</v>
       </c>
@@ -1696,10 +2156,18 @@
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
+      <c r="A45" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E45" s="3">
         <v>0.33680555555555558</v>
       </c>
@@ -1728,10 +2196,18 @@
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
+      <c r="A47" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E47" s="3">
         <v>0.30902777777777779</v>
       </c>
@@ -1740,10 +2216,18 @@
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
+      <c r="A48" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E48" s="3">
         <v>0.3125</v>
       </c>
@@ -1752,10 +2236,18 @@
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
+      <c r="A49" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E49" s="3">
         <v>0.31597222222222221</v>
       </c>
@@ -1764,10 +2256,18 @@
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
+      <c r="A50" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E50" s="3">
         <v>0.33680555555555558</v>
       </c>
@@ -1776,10 +2276,18 @@
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
+      <c r="A51" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E51" s="3">
         <v>0.34027777777777773</v>
       </c>
@@ -1808,10 +2316,18 @@
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
+      <c r="A53" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E53" s="3">
         <v>0.30902777777777779</v>
       </c>
@@ -1820,10 +2336,18 @@
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
+      <c r="A54" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E54" s="3">
         <v>0.3125</v>
       </c>
@@ -1832,10 +2356,18 @@
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
+      <c r="A55" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E55" s="3">
         <v>0.32291666666666669</v>
       </c>
@@ -1844,10 +2376,18 @@
       </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
+      <c r="A56" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E56" s="3">
         <v>0.33333333333333331</v>
       </c>
@@ -1876,10 +2416,18 @@
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="7"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
+      <c r="A58" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E58" s="3">
         <v>0.2986111111111111</v>
       </c>
@@ -1888,10 +2436,18 @@
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
+      <c r="A59" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E59" s="3">
         <v>0.30555555555555552</v>
       </c>
@@ -1900,10 +2456,18 @@
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
+      <c r="A60" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E60" s="3">
         <v>0.30902777777777779</v>
       </c>
@@ -1912,10 +2476,18 @@
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
+      <c r="A61" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E61" s="3">
         <v>0.3125</v>
       </c>
@@ -1944,10 +2516,18 @@
       </c>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
+      <c r="A63" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E63" s="3">
         <v>0.29652777777777778</v>
       </c>
@@ -1956,10 +2536,18 @@
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
+      <c r="A64" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E64" s="3">
         <v>0.30208333333333331</v>
       </c>
@@ -1968,10 +2556,18 @@
       </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
+      <c r="A65" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E65" s="3">
         <v>0.31597222222222221</v>
       </c>
@@ -1980,10 +2576,18 @@
       </c>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
+      <c r="A66" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E66" s="3">
         <v>0.32291666666666669</v>
       </c>
@@ -1992,10 +2596,18 @@
       </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
+      <c r="A67" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E67" s="3">
         <v>0.3263888888888889</v>
       </c>
@@ -2004,10 +2616,18 @@
       </c>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
+      <c r="A68" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E68" s="3">
         <v>0.33333333333333331</v>
       </c>
@@ -2016,10 +2636,18 @@
       </c>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
+      <c r="A69" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E69" s="3">
         <v>0.33680555555555558</v>
       </c>
@@ -2028,10 +2656,18 @@
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
+      <c r="A70" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E70" s="3">
         <v>0.34375</v>
       </c>
@@ -2060,10 +2696,18 @@
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="7"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
+      <c r="A72" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E72" s="3">
         <v>0.3</v>
       </c>
@@ -2072,10 +2716,18 @@
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
+      <c r="A73" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E73" s="3">
         <v>0.30416666666666664</v>
       </c>
@@ -2084,10 +2736,18 @@
       </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="7"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
+      <c r="A74" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E74" s="3">
         <v>0.31597222222222221</v>
       </c>
@@ -2096,10 +2756,18 @@
       </c>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="7"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
+      <c r="A75" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E75" s="3">
         <v>0.31944444444444448</v>
       </c>
@@ -2108,10 +2776,18 @@
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="7"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
+      <c r="A76" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E76" s="3">
         <v>0.3215277777777778</v>
       </c>
@@ -2120,10 +2796,18 @@
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
+      <c r="A77" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E77" s="3">
         <v>0.32500000000000001</v>
       </c>
@@ -2132,10 +2816,18 @@
       </c>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="7"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
+      <c r="A78" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E78" s="3">
         <v>0.3263888888888889</v>
       </c>
@@ -2144,10 +2836,18 @@
       </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="7"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
+      <c r="A79" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E79" s="3">
         <v>0.3298611111111111</v>
       </c>
@@ -2156,10 +2856,18 @@
       </c>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="7"/>
-      <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="7"/>
+      <c r="A80" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E80" s="3">
         <v>0.33680555555555558</v>
       </c>
@@ -2188,10 +2896,18 @@
       </c>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="7"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="7"/>
+      <c r="A82" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E82" s="3">
         <v>0.2986111111111111</v>
       </c>
@@ -2200,10 +2916,18 @@
       </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="7"/>
-      <c r="B83" s="7"/>
-      <c r="C83" s="7"/>
-      <c r="D83" s="7"/>
+      <c r="A83" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E83" s="3">
         <v>0.30208333333333331</v>
       </c>
@@ -2212,10 +2936,18 @@
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="7"/>
-      <c r="B84" s="7"/>
-      <c r="C84" s="7"/>
-      <c r="D84" s="7"/>
+      <c r="A84" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E84" s="3">
         <v>0.30902777777777779</v>
       </c>
@@ -2224,10 +2956,18 @@
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="A85" s="7"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="7"/>
-      <c r="D85" s="7"/>
+      <c r="A85" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E85" s="3">
         <v>0.3125</v>
       </c>
@@ -2236,10 +2976,18 @@
       </c>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" s="7"/>
-      <c r="B86" s="7"/>
-      <c r="C86" s="7"/>
-      <c r="D86" s="7"/>
+      <c r="A86" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E86" s="3">
         <v>0.31597222222222221</v>
       </c>
@@ -2248,10 +2996,18 @@
       </c>
     </row>
     <row r="87" spans="1:6">
-      <c r="A87" s="7"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
-      <c r="D87" s="7"/>
+      <c r="A87" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E87" s="3">
         <v>0.31805555555555554</v>
       </c>
@@ -2260,10 +3016,18 @@
       </c>
     </row>
     <row r="88" spans="1:6">
-      <c r="A88" s="7"/>
-      <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
-      <c r="D88" s="7"/>
+      <c r="A88" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E88" s="3">
         <v>0.31944444444444448</v>
       </c>
@@ -2292,10 +3056,18 @@
       </c>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="7"/>
-      <c r="B90" s="7"/>
-      <c r="C90" s="7"/>
-      <c r="D90" s="7"/>
+      <c r="A90" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E90" s="3">
         <v>0.30902777777777779</v>
       </c>
@@ -2304,10 +3076,18 @@
       </c>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="7"/>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="7"/>
+      <c r="A91" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E91" s="3">
         <v>0.31597222222222221</v>
       </c>
@@ -2316,10 +3096,18 @@
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="7"/>
-      <c r="B92" s="7"/>
-      <c r="C92" s="7"/>
-      <c r="D92" s="7"/>
+      <c r="A92" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E92" s="3">
         <v>0.31944444444444448</v>
       </c>
@@ -2328,10 +3116,18 @@
       </c>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="7"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="7"/>
-      <c r="D93" s="7"/>
+      <c r="A93" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E93" s="3">
         <v>0.32222222222222224</v>
       </c>
@@ -2340,10 +3136,18 @@
       </c>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="7"/>
-      <c r="B94" s="7"/>
-      <c r="C94" s="7"/>
-      <c r="D94" s="7"/>
+      <c r="A94" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E94" s="3">
         <v>0.3263888888888889</v>
       </c>
@@ -2352,10 +3156,18 @@
       </c>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" s="7"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="7"/>
+      <c r="A95" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E95" s="3">
         <v>0.32916666666666666</v>
       </c>
@@ -2364,10 +3176,18 @@
       </c>
     </row>
     <row r="96" spans="1:6">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7"/>
+      <c r="A96" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="E96" s="3">
         <v>0.33194444444444443</v>
       </c>
@@ -2396,10 +3216,18 @@
       </c>
     </row>
     <row r="98" spans="1:6">
-      <c r="A98" s="7"/>
-      <c r="B98" s="7"/>
-      <c r="C98" s="7"/>
-      <c r="D98" s="7"/>
+      <c r="A98" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>236</v>
+      </c>
       <c r="E98" s="3">
         <v>0.28125</v>
       </c>
@@ -2408,10 +3236,18 @@
       </c>
     </row>
     <row r="99" spans="1:6">
-      <c r="A99" s="7"/>
-      <c r="B99" s="7"/>
-      <c r="C99" s="7"/>
-      <c r="D99" s="7"/>
+      <c r="A99" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>236</v>
+      </c>
       <c r="E99" s="3">
         <v>0.28333333333333333</v>
       </c>
@@ -2420,10 +3256,18 @@
       </c>
     </row>
     <row r="100" spans="1:6">
-      <c r="A100" s="7"/>
-      <c r="B100" s="7"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="7"/>
+      <c r="A100" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>236</v>
+      </c>
       <c r="E100" s="3">
         <v>0.28472222222222221</v>
       </c>
@@ -2432,10 +3276,18 @@
       </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="7"/>
-      <c r="B101" s="7"/>
-      <c r="C101" s="7"/>
-      <c r="D101" s="7"/>
+      <c r="A101" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>236</v>
+      </c>
       <c r="E101" s="3">
         <v>0.28819444444444448</v>
       </c>
@@ -2444,10 +3296,18 @@
       </c>
     </row>
     <row r="102" spans="1:6">
-      <c r="A102" s="7"/>
-      <c r="B102" s="7"/>
-      <c r="C102" s="7"/>
-      <c r="D102" s="7"/>
+      <c r="A102" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>236</v>
+      </c>
       <c r="E102" s="3">
         <v>0.2951388888888889</v>
       </c>
@@ -2456,10 +3316,18 @@
       </c>
     </row>
     <row r="103" spans="1:6">
-      <c r="A103" s="7"/>
-      <c r="B103" s="7"/>
-      <c r="C103" s="7"/>
-      <c r="D103" s="7"/>
+      <c r="A103" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>236</v>
+      </c>
       <c r="E103" s="3">
         <v>0.30208333333333331</v>
       </c>
@@ -2468,10 +3336,18 @@
       </c>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" s="7"/>
-      <c r="B104" s="7"/>
-      <c r="C104" s="7"/>
-      <c r="D104" s="7"/>
+      <c r="A104" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>236</v>
+      </c>
       <c r="E104" s="3">
         <v>0.30555555555555552</v>
       </c>
@@ -2480,10 +3356,18 @@
       </c>
     </row>
     <row r="105" spans="1:6">
-      <c r="A105" s="7"/>
-      <c r="B105" s="7"/>
-      <c r="C105" s="7"/>
-      <c r="D105" s="7"/>
+      <c r="A105" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>236</v>
+      </c>
       <c r="E105" s="3">
         <v>0.31944444444444448</v>
       </c>
@@ -2492,10 +3376,18 @@
       </c>
     </row>
     <row r="106" spans="1:6">
-      <c r="A106" s="7"/>
-      <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="7"/>
+      <c r="A106" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>236</v>
+      </c>
       <c r="E106" s="3">
         <v>0.3263888888888889</v>
       </c>
@@ -2504,10 +3396,18 @@
       </c>
     </row>
     <row r="107" spans="1:6">
-      <c r="A107" s="7"/>
-      <c r="B107" s="7"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="7"/>
+      <c r="A107" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>236</v>
+      </c>
       <c r="E107" s="3">
         <v>0.33333333333333331</v>
       </c>
@@ -2536,10 +3436,18 @@
       </c>
     </row>
     <row r="109" spans="1:6">
-      <c r="A109" s="7"/>
-      <c r="B109" s="7"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="7"/>
+      <c r="A109" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>189</v>
+      </c>
       <c r="E109" s="3">
         <v>0.26597222222222222</v>
       </c>
@@ -2548,10 +3456,18 @@
       </c>
     </row>
     <row r="110" spans="1:6">
-      <c r="A110" s="7"/>
-      <c r="B110" s="7"/>
-      <c r="C110" s="7"/>
-      <c r="D110" s="7"/>
+      <c r="A110" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>189</v>
+      </c>
       <c r="E110" s="3">
         <v>0.2673611111111111</v>
       </c>
@@ -2560,10 +3476,18 @@
       </c>
     </row>
     <row r="111" spans="1:6">
-      <c r="A111" s="7"/>
-      <c r="B111" s="7"/>
-      <c r="C111" s="7"/>
-      <c r="D111" s="7"/>
+      <c r="A111" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>189</v>
+      </c>
       <c r="E111" s="3">
         <v>0.28472222222222221</v>
       </c>
@@ -2572,10 +3496,18 @@
       </c>
     </row>
     <row r="112" spans="1:6">
-      <c r="A112" s="7"/>
-      <c r="B112" s="7"/>
-      <c r="C112" s="7"/>
-      <c r="D112" s="7"/>
+      <c r="A112" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>189</v>
+      </c>
       <c r="E112" s="3">
         <v>0.31944444444444448</v>
       </c>
@@ -2604,10 +3536,18 @@
       </c>
     </row>
     <row r="114" spans="1:6">
-      <c r="A114" s="7"/>
-      <c r="B114" s="7"/>
-      <c r="C114" s="7"/>
-      <c r="D114" s="7"/>
+      <c r="A114" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D114" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E114" s="3">
         <v>0.28472222222222221</v>
       </c>
@@ -2616,10 +3556,18 @@
       </c>
     </row>
     <row r="115" spans="1:6">
-      <c r="A115" s="7"/>
-      <c r="B115" s="7"/>
-      <c r="C115" s="7"/>
-      <c r="D115" s="7"/>
+      <c r="A115" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D115" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E115" s="3">
         <v>0.2951388888888889</v>
       </c>
@@ -2628,10 +3576,18 @@
       </c>
     </row>
     <row r="116" spans="1:6">
-      <c r="A116" s="7"/>
-      <c r="B116" s="7"/>
-      <c r="C116" s="7"/>
-      <c r="D116" s="7"/>
+      <c r="A116" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D116" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E116" s="3">
         <v>0.30902777777777779</v>
       </c>
@@ -2660,10 +3616,18 @@
       </c>
     </row>
     <row r="118" spans="1:6">
-      <c r="A118" s="7"/>
-      <c r="B118" s="7"/>
-      <c r="C118" s="7"/>
-      <c r="D118" s="7"/>
+      <c r="A118" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D118" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E118" s="3">
         <v>0.2673611111111111</v>
       </c>
@@ -2672,10 +3636,18 @@
       </c>
     </row>
     <row r="119" spans="1:6">
-      <c r="A119" s="7"/>
-      <c r="B119" s="7"/>
-      <c r="C119" s="7"/>
-      <c r="D119" s="7"/>
+      <c r="A119" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D119" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E119" s="3">
         <v>0.28125</v>
       </c>
@@ -2684,10 +3656,18 @@
       </c>
     </row>
     <row r="120" spans="1:6">
-      <c r="A120" s="7"/>
-      <c r="B120" s="7"/>
-      <c r="C120" s="7"/>
-      <c r="D120" s="7"/>
+      <c r="A120" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E120" s="3">
         <v>0.29166666666666669</v>
       </c>
@@ -2696,10 +3676,18 @@
       </c>
     </row>
     <row r="121" spans="1:6">
-      <c r="A121" s="7"/>
-      <c r="B121" s="7"/>
-      <c r="C121" s="7"/>
-      <c r="D121" s="7"/>
+      <c r="A121" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="E121" s="3">
         <v>0.30555555555555552</v>
       </c>
@@ -2708,84 +3696,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="A117:A121"/>
-    <mergeCell ref="B117:B121"/>
-    <mergeCell ref="C117:C121"/>
-    <mergeCell ref="D117:D121"/>
-    <mergeCell ref="D108:D112"/>
-    <mergeCell ref="A108:A112"/>
-    <mergeCell ref="B108:B112"/>
-    <mergeCell ref="C108:C112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="B113:B116"/>
-    <mergeCell ref="C113:C116"/>
-    <mergeCell ref="D113:D116"/>
-    <mergeCell ref="A89:A96"/>
-    <mergeCell ref="B89:B96"/>
-    <mergeCell ref="C89:C96"/>
-    <mergeCell ref="D89:D96"/>
-    <mergeCell ref="A97:A107"/>
-    <mergeCell ref="B97:B107"/>
-    <mergeCell ref="C97:C107"/>
-    <mergeCell ref="D97:D107"/>
-    <mergeCell ref="A71:A80"/>
-    <mergeCell ref="B71:B80"/>
-    <mergeCell ref="C71:C80"/>
-    <mergeCell ref="D71:D80"/>
-    <mergeCell ref="A81:A88"/>
-    <mergeCell ref="B81:B88"/>
-    <mergeCell ref="C81:C88"/>
-    <mergeCell ref="D81:D88"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="C57:C61"/>
-    <mergeCell ref="D57:D61"/>
-    <mergeCell ref="A62:A70"/>
-    <mergeCell ref="B62:B70"/>
-    <mergeCell ref="D62:D70"/>
-    <mergeCell ref="C62:C70"/>
-    <mergeCell ref="A46:A51"/>
-    <mergeCell ref="B46:B51"/>
-    <mergeCell ref="C46:C51"/>
-    <mergeCell ref="D46:D51"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="D52:D56"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="C34:C39"/>
-    <mergeCell ref="D34:D39"/>
-    <mergeCell ref="A40:A45"/>
-    <mergeCell ref="B40:B45"/>
-    <mergeCell ref="C40:C45"/>
-    <mergeCell ref="D40:D45"/>
-    <mergeCell ref="D24:D29"/>
-    <mergeCell ref="C24:C29"/>
-    <mergeCell ref="B24:B29"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="C11:C17"/>
-    <mergeCell ref="D11:D17"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="C5:C10"/>
-    <mergeCell ref="D5:D10"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Shuttle Routes. Fixed some address
</commit_message>
<xml_diff>
--- a/shuttle.xlsx
+++ b/shuttle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangwentao/Desktop/浦东公租房/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2223943D-31B6-0649-8C5E-0F66E6747915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8C2BA4-AE66-EE47-AFCE-897C5394DE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" xr2:uid="{C9FD647D-2FFF-4BC2-B220-0407C10CAB3A}"/>
   </bookViews>
@@ -98,10 +98,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>通河路共江路/共康八村公交站</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>共和新路闻喜路公交站</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -398,9 +394,6 @@
     <t>广粤路奎照路公交站</t>
   </si>
   <si>
-    <t>万安路逸仙路公交站</t>
-  </si>
-  <si>
     <t>大木桥路茶陵路公交站</t>
   </si>
   <si>
@@ -494,15 +487,9 @@
     <t>上南路康沈路公交站</t>
   </si>
   <si>
-    <t>沪南路上南路公交站</t>
-  </si>
-  <si>
     <t>沪南公路秀浦路公交站</t>
   </si>
   <si>
-    <t>沪南路康花路(东郊百联）公交站</t>
-  </si>
-  <si>
     <t>龙阳路地铁站公交站</t>
   </si>
   <si>
@@ -623,9 +610,6 @@
     <t>兰坪路江川路(高华小区)公交站</t>
   </si>
   <si>
-    <t>安宁路二街坊门口公交站</t>
-  </si>
-  <si>
     <t>东川路碧江路公交站</t>
   </si>
   <si>
@@ -852,6 +836,21 @@
   </si>
   <si>
     <t>沪EB7900</t>
+  </si>
+  <si>
+    <t>沪南公路上南路公交站</t>
+  </si>
+  <si>
+    <t>沪南路康花路公交站</t>
+  </si>
+  <si>
+    <t>安宁路26弄</t>
+  </si>
+  <si>
+    <t>万安路逸仙路</t>
+  </si>
+  <si>
+    <t>通河路共江路公交站</t>
   </si>
 </sst>
 </file>
@@ -919,7 +918,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -940,9 +939,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1262,7 +1258,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -1289,2410 +1285,2410 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="3">
         <v>0.29166666666666669</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>189</v>
+      <c r="A3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="E3" s="3">
         <v>0.30555555555555552</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>189</v>
+      <c r="A4" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="E4" s="3">
         <v>0.3125</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="3">
         <v>0.28472222222222221</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>193</v>
+      <c r="A6" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E6" s="3">
         <v>0.29166666666666669</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>193</v>
+      <c r="A7" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E7" s="3">
         <v>0.30555555555555552</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>193</v>
+      <c r="A8" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E8" s="3">
         <v>0.30902777777777779</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>193</v>
+      <c r="A9" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E9" s="3">
         <v>0.3125</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>193</v>
+      <c r="A10" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E10" s="3">
         <v>0.31597222222222221</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="3">
         <v>0.29166666666666669</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>193</v>
+      <c r="A12" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E12" s="3">
         <v>0.29375000000000001</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>15</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>193</v>
+      <c r="A13" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E13" s="3">
         <v>0.2951388888888889</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>193</v>
+      <c r="A14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E14" s="3">
         <v>0.2986111111111111</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>193</v>
+      <c r="A15" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E15" s="3">
         <v>0.30208333333333331</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>193</v>
+      <c r="A16" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E16" s="3">
         <v>0.30902777777777779</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>193</v>
+      <c r="A17" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E17" s="3">
         <v>0.31944444444444448</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>94</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="3">
         <v>0.31597222222222221</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="A19" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>193</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E19" s="3">
         <v>0.31944444444444448</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D20" s="7" t="s">
+      <c r="A20" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>193</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E20" s="3">
         <v>0.32291666666666669</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D21" s="7" t="s">
+      <c r="A21" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>193</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E21" s="3">
         <v>0.3263888888888889</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="A22" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>193</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E22" s="3">
         <v>0.33333333333333331</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D23" s="7" t="s">
+      <c r="A23" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>193</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E23" s="3">
         <v>0.34027777777777773</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="C24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="3">
         <v>0.30208333333333331</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>193</v>
+      <c r="A25" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E25" s="3">
         <v>0.30555555555555552</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>193</v>
+      <c r="A26" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E26" s="3">
         <v>0.3125</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>193</v>
+      <c r="A27" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E27" s="3">
         <v>0.31944444444444448</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>193</v>
+      <c r="A28" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E28" s="3">
         <v>0.3263888888888889</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>193</v>
+      <c r="A29" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E29" s="3">
         <v>0.33333333333333331</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="3">
         <v>0.29166666666666669</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>193</v>
+      <c r="A31" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E31" s="3">
         <v>0.30555555555555552</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>193</v>
+      <c r="A32" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E32" s="3">
         <v>0.31597222222222221</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>193</v>
+      <c r="A33" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E33" s="3">
         <v>0.31944444444444448</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="C34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="3">
         <v>0.29166666666666669</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>193</v>
+      <c r="A35" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E35" s="3">
         <v>0.30555555555555552</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>193</v>
+      <c r="A36" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E36" s="3">
         <v>0.30902777777777779</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>193</v>
+      <c r="A37" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E37" s="3">
         <v>0.3125</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>193</v>
+      <c r="A38" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E38" s="3">
         <v>0.3263888888888889</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>193</v>
+      <c r="A39" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E39" s="3">
         <v>0.3298611111111111</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="C40" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="3">
         <v>0.30555555555555552</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>193</v>
+      <c r="A41" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E41" s="3">
         <v>0.31944444444444448</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>193</v>
+      <c r="A42" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E42" s="3">
         <v>0.3215277777777778</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>193</v>
+      <c r="A43" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E43" s="3">
         <v>0.32500000000000001</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>193</v>
+      <c r="A44" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E44" s="3">
         <v>0.33333333333333331</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>193</v>
+      <c r="A45" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E45" s="3">
         <v>0.33680555555555558</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="C46" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E46" s="3">
         <v>0.2986111111111111</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>193</v>
+      <c r="A47" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E47" s="3">
         <v>0.30902777777777779</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>193</v>
+      <c r="A48" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E48" s="3">
         <v>0.3125</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>193</v>
+      <c r="A49" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E49" s="3">
         <v>0.31597222222222221</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>193</v>
+      <c r="A50" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E50" s="3">
         <v>0.33680555555555558</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>193</v>
+      <c r="A51" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E51" s="3">
         <v>0.34027777777777773</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="C52" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="3">
         <v>0.30555555555555552</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>193</v>
+      <c r="A53" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E53" s="3">
         <v>0.30902777777777779</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>126</v>
+        <v>241</v>
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>193</v>
+      <c r="A54" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E54" s="3">
         <v>0.3125</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>193</v>
+      <c r="A55" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E55" s="3">
         <v>0.32291666666666669</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>128</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>193</v>
+      <c r="A56" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E56" s="3">
         <v>0.33333333333333331</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="C57" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C57" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E57" s="3">
         <v>0.29166666666666669</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>193</v>
+      <c r="A58" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E58" s="3">
         <v>0.2986111111111111</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>193</v>
+      <c r="A59" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E59" s="3">
         <v>0.30555555555555552</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>193</v>
+      <c r="A60" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E60" s="3">
         <v>0.30902777777777779</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>193</v>
+      <c r="A61" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E61" s="3">
         <v>0.3125</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="C62" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C62" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>49</v>
+      <c r="D62" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E62" s="3">
         <v>0.2951388888888889</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>48</v>
+      <c r="A63" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E63" s="3">
         <v>0.29652777777777778</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>48</v>
+      <c r="A64" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E64" s="3">
         <v>0.30208333333333331</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>48</v>
+      <c r="A65" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E65" s="3">
         <v>0.31597222222222221</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>48</v>
+      <c r="A66" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E66" s="3">
         <v>0.32291666666666669</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>48</v>
+      <c r="A67" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E67" s="3">
         <v>0.3263888888888889</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>48</v>
+      <c r="A68" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E68" s="3">
         <v>0.33333333333333331</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>48</v>
+      <c r="A69" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E69" s="3">
         <v>0.33680555555555558</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>48</v>
+      <c r="A70" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E70" s="3">
         <v>0.34375</v>
       </c>
       <c r="F70" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="7" t="s">
+      <c r="B71" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="C71" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C71" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>49</v>
+      <c r="D71" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E71" s="3">
         <v>0.2986111111111111</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>48</v>
+      <c r="A72" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E72" s="3">
         <v>0.3</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>48</v>
+      <c r="A73" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E73" s="3">
         <v>0.30416666666666664</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>48</v>
+      <c r="A74" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E74" s="3">
         <v>0.31597222222222221</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>48</v>
+      <c r="A75" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E75" s="3">
         <v>0.31944444444444448</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>48</v>
+      <c r="A76" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E76" s="3">
         <v>0.3215277777777778</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>48</v>
+      <c r="A77" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E77" s="3">
         <v>0.32500000000000001</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>48</v>
+      <c r="A78" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E78" s="3">
         <v>0.3263888888888889</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>48</v>
+      <c r="A79" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E79" s="3">
         <v>0.3298611111111111</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>48</v>
+      <c r="A80" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E80" s="3">
         <v>0.33680555555555558</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:6">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="C81" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C81" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>49</v>
+      <c r="D81" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E81" s="3">
         <v>0.29166666666666669</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>48</v>
+      <c r="A82" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E82" s="3">
         <v>0.2986111111111111</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>48</v>
+      <c r="A83" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E83" s="3">
         <v>0.30208333333333331</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>48</v>
+      <c r="A84" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E84" s="3">
         <v>0.30902777777777779</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="A85" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>48</v>
+      <c r="A85" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E85" s="3">
         <v>0.3125</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>48</v>
+      <c r="A86" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E86" s="3">
         <v>0.31597222222222221</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="87" spans="1:6">
-      <c r="A87" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>48</v>
+      <c r="A87" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E87" s="3">
         <v>0.31805555555555554</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="88" spans="1:6">
-      <c r="A88" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>48</v>
+      <c r="A88" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E88" s="3">
         <v>0.31944444444444448</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="C89" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C89" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>48</v>
+      <c r="D89" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E89" s="3">
         <v>0.30208333333333331</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>48</v>
+      <c r="A90" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E90" s="3">
         <v>0.30902777777777779</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>48</v>
+      <c r="A91" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E91" s="3">
         <v>0.31597222222222221</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>48</v>
+      <c r="A92" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E92" s="3">
         <v>0.31944444444444448</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>48</v>
+      <c r="A93" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E93" s="3">
         <v>0.32222222222222224</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>48</v>
+      <c r="A94" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E94" s="3">
         <v>0.3263888888888889</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>48</v>
+      <c r="A95" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E95" s="3">
         <v>0.32916666666666666</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="96" spans="1:6">
-      <c r="A96" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B96" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>48</v>
+      <c r="A96" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E96" s="3">
         <v>0.33194444444444443</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="97" spans="1:6">
-      <c r="A97" s="7" t="s">
+      <c r="A97" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B97" s="7" t="s">
+      <c r="C97" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C97" s="7" t="s">
+      <c r="D97" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="E97" s="3">
         <v>0.27777777777777779</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="98" spans="1:6">
-      <c r="A98" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D98" s="7" t="s">
-        <v>236</v>
+      <c r="A98" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="E98" s="3">
         <v>0.28125</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>169</v>
+        <v>243</v>
       </c>
     </row>
     <row r="99" spans="1:6">
-      <c r="A99" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>236</v>
+      <c r="A99" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="E99" s="3">
         <v>0.28333333333333333</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="100" spans="1:6">
-      <c r="A100" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D100" s="7" t="s">
-        <v>236</v>
+      <c r="A100" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="E100" s="3">
         <v>0.28472222222222221</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B101" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D101" s="7" t="s">
-        <v>236</v>
+      <c r="A101" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="E101" s="3">
         <v>0.28819444444444448</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="102" spans="1:6">
-      <c r="A102" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D102" s="7" t="s">
-        <v>236</v>
+      <c r="A102" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="E102" s="3">
         <v>0.2951388888888889</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="103" spans="1:6">
-      <c r="A103" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B103" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C103" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D103" s="7" t="s">
-        <v>236</v>
+      <c r="A103" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="E103" s="3">
         <v>0.30208333333333331</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C104" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D104" s="7" t="s">
-        <v>236</v>
+      <c r="A104" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="E104" s="3">
         <v>0.30555555555555552</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:6">
-      <c r="A105" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D105" s="7" t="s">
-        <v>236</v>
+      <c r="A105" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="E105" s="3">
         <v>0.31944444444444448</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="106" spans="1:6">
-      <c r="A106" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B106" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>236</v>
+      <c r="A106" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="E106" s="3">
         <v>0.3263888888888889</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="107" spans="1:6">
-      <c r="A107" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B107" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D107" s="7" t="s">
-        <v>236</v>
+      <c r="A107" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="E107" s="3">
         <v>0.33333333333333331</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="108" spans="1:6">
-      <c r="A108" s="7" t="s">
+      <c r="A108" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B108" s="7" t="s">
+      <c r="C108" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C108" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D108" s="7" t="s">
+      <c r="D108" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E108" s="3">
         <v>0.2638888888888889</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="109" spans="1:6">
-      <c r="A109" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="B109" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="C109" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="D109" s="7" t="s">
-        <v>189</v>
+      <c r="A109" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="E109" s="3">
         <v>0.26597222222222222</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="110" spans="1:6">
-      <c r="A110" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="D110" s="7" t="s">
-        <v>189</v>
+      <c r="A110" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="E110" s="3">
         <v>0.2673611111111111</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="111" spans="1:6">
-      <c r="A111" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="D111" s="7" t="s">
-        <v>189</v>
+      <c r="A111" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="E111" s="3">
         <v>0.28472222222222221</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="112" spans="1:6">
-      <c r="A112" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="B112" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="C112" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="D112" s="7" t="s">
-        <v>189</v>
+      <c r="A112" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="E112" s="3">
         <v>0.31944444444444448</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="1:6">
-      <c r="A113" s="7" t="s">
+      <c r="A113" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B113" s="7" t="s">
+      <c r="C113" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C113" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D113" s="7" t="s">
+      <c r="D113" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E113" s="3">
         <v>0.27777777777777779</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="114" spans="1:6">
-      <c r="A114" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="B114" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="D114" s="7" t="s">
-        <v>193</v>
+      <c r="A114" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E114" s="3">
         <v>0.28472222222222221</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="115" spans="1:6">
-      <c r="A115" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="B115" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="C115" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="D115" s="7" t="s">
-        <v>193</v>
+      <c r="A115" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E115" s="3">
         <v>0.2951388888888889</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="116" spans="1:6">
-      <c r="A116" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="B116" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="C116" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="D116" s="7" t="s">
-        <v>193</v>
+      <c r="A116" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E116" s="3">
         <v>0.30902777777777779</v>
       </c>
       <c r="F116" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="117" spans="1:6">
-      <c r="A117" s="7" t="s">
+      <c r="B117" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B117" s="7" t="s">
+      <c r="C117" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C117" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D117" s="7" t="s">
+      <c r="D117" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E117" s="3">
         <v>0.26041666666666669</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="118" spans="1:6">
-      <c r="A118" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="B118" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C118" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="D118" s="7" t="s">
-        <v>193</v>
+      <c r="A118" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E118" s="3">
         <v>0.2673611111111111</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="119" spans="1:6">
-      <c r="A119" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="D119" s="7" t="s">
-        <v>193</v>
+      <c r="A119" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E119" s="3">
         <v>0.28125</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="120" spans="1:6">
-      <c r="A120" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="B120" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C120" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="D120" s="7" t="s">
-        <v>193</v>
+      <c r="A120" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E120" s="3">
         <v>0.29166666666666669</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="121" spans="1:6">
-      <c r="A121" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="B121" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C121" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="D121" s="7" t="s">
-        <v>193</v>
+      <c r="A121" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E121" s="3">
         <v>0.30555555555555552</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>